<commit_message>
finished graphs + storytelling
</commit_message>
<xml_diff>
--- a/data/Antalet studerande i YH inom olika utbildningsområden 2012-2024.xlsx
+++ b/data/Antalet studerande i YH inom olika utbildningsområden 2012-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freja\Desktop\Gruppprojekt_datavisualisering\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C118D276-DB51-4F73-B8E1-7B3E94E25CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184528C2-8AAA-4CD5-BE11-304B5A5903BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="492" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="000004ZO" sheetId="2" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
-  <si>
-    <t>Totalt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Data/It</t>
   </si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>Transporttjänster</t>
-  </si>
-  <si>
-    <t>Övrigt</t>
   </si>
   <si>
     <t>2005</t>
@@ -497,73 +491,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>2587</v>
@@ -584,7 +572,7 @@
         <v>114</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2">
         <v>2803</v>
@@ -607,16 +595,10 @@
       <c r="O2" s="2">
         <v>822</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>24789</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>2546</v>
@@ -660,16 +642,10 @@
       <c r="O3" s="2">
         <v>1104</v>
       </c>
-      <c r="P3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>29556</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>2797</v>
@@ -713,16 +689,10 @@
       <c r="O4" s="2">
         <v>1357</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>33684</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>2817</v>
@@ -766,16 +736,10 @@
       <c r="O5" s="2">
         <v>1590</v>
       </c>
-      <c r="P5" s="2">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>36657</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>2857</v>
@@ -819,16 +783,10 @@
       <c r="O6" s="2">
         <v>1696</v>
       </c>
-      <c r="P6" s="2">
-        <v>59</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>39417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>2903</v>
@@ -872,16 +830,10 @@
       <c r="O7" s="2">
         <v>1859</v>
       </c>
-      <c r="P7" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>41597</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>3160</v>
@@ -925,16 +877,10 @@
       <c r="O8" s="2">
         <v>1845</v>
       </c>
-      <c r="P8" s="2">
-        <v>99</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>3398</v>
@@ -978,16 +924,10 @@
       <c r="O9" s="2">
         <v>1487</v>
       </c>
-      <c r="P9" s="2">
-        <v>174</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>40754</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <v>4054</v>
@@ -1031,16 +971,10 @@
       <c r="O10" s="2">
         <v>1116</v>
       </c>
-      <c r="P10" s="2">
-        <v>224</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>42596</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
         <v>4937</v>
@@ -1084,16 +1018,10 @@
       <c r="O11" s="2">
         <v>941</v>
       </c>
-      <c r="P11" s="2">
-        <v>248</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>44929</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>5812</v>
@@ -1137,16 +1065,10 @@
       <c r="O12" s="2">
         <v>1190</v>
       </c>
-      <c r="P12" s="2">
-        <v>247</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>46633</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>6183</v>
@@ -1190,16 +1112,10 @@
       <c r="O13" s="2">
         <v>1544</v>
       </c>
-      <c r="P13" s="2">
-        <v>259</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>47983</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <v>6210</v>
@@ -1243,16 +1159,10 @@
       <c r="O14" s="2">
         <v>1850</v>
       </c>
-      <c r="P14" s="2">
-        <v>282</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>50373</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
         <v>5704</v>
@@ -1296,16 +1206,10 @@
       <c r="O15" s="2">
         <v>1749</v>
       </c>
-      <c r="P15" s="2">
-        <v>257</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>52741</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <v>7086</v>
@@ -1349,16 +1253,10 @@
       <c r="O16" s="2">
         <v>1673</v>
       </c>
-      <c r="P16" s="2">
-        <v>323</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>61393</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <v>10283</v>
@@ -1402,16 +1300,10 @@
       <c r="O17" s="2">
         <v>1757</v>
       </c>
-      <c r="P17" s="2">
-        <v>426</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>75371</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>12852</v>
@@ -1455,16 +1347,10 @@
       <c r="O18" s="2">
         <v>1573</v>
       </c>
-      <c r="P18" s="2">
-        <v>477</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>82753</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <v>14255</v>
@@ -1508,16 +1394,10 @@
       <c r="O19" s="2">
         <v>1490</v>
       </c>
-      <c r="P19" s="2">
-        <v>515</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>84871</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <v>15162</v>
@@ -1561,16 +1441,10 @@
       <c r="O20" s="2">
         <v>1618</v>
       </c>
-      <c r="P20" s="2">
-        <v>433</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>84560</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <v>16447</v>
@@ -1613,12 +1487,6 @@
       </c>
       <c r="O21" s="2">
         <v>1691</v>
-      </c>
-      <c r="P21" s="2">
-        <v>371</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>87225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>